<commit_message>
the  schulerliste wurde geändert
</commit_message>
<xml_diff>
--- a/schuelerliste.xlsx
+++ b/schuelerliste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Workspace\bg-school-certificate-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC2B60D-175A-4D43-9B9D-CE7C16E89ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0222185C-952C-4137-B10B-D6F6C1F716D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10695" yWindow="3015" windowWidth="38700" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,45 +25,108 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
-  <si>
-    <t>Familienname</t>
-  </si>
-  <si>
-    <t>Vorname_Elternteil</t>
-  </si>
-  <si>
-    <t>Vorname_Kind</t>
-  </si>
-  <si>
-    <t>Mustermann</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Anna</t>
-  </si>
-  <si>
-    <t>Felix</t>
-  </si>
-  <si>
-    <t>Schmidt</t>
-  </si>
-  <si>
-    <t>Julia</t>
-  </si>
-  <si>
-    <t>Leon</t>
-  </si>
-  <si>
-    <t>Bauer</t>
-  </si>
-  <si>
-    <t>Thomas</t>
-  </si>
-  <si>
-    <t>Sophie</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+  <si>
+    <t>Mitglied</t>
+  </si>
+  <si>
+    <t>Kind</t>
+  </si>
+  <si>
+    <t>Klasse</t>
+  </si>
+  <si>
+    <t>Eltern2</t>
+  </si>
+  <si>
+    <t>Gezahlt</t>
+  </si>
+  <si>
+    <t>Gezahlt Details</t>
+  </si>
+  <si>
+    <t>Anzahl Kinder</t>
+  </si>
+  <si>
+    <t>Zahlungszeilen</t>
+  </si>
+  <si>
+    <t>Freiham Klasse 4b</t>
+  </si>
+  <si>
+    <t>Freiham Klasse 9b</t>
+  </si>
+  <si>
+    <t>Freiham PUG 2</t>
+  </si>
+  <si>
+    <t>540.00 (180.00+180.00+180.00)</t>
+  </si>
+  <si>
+    <t>339, 621, 647</t>
+  </si>
+  <si>
+    <t>Valentin Trifonov</t>
+  </si>
+  <si>
+    <t>Neubiberg Klasse 4a</t>
+  </si>
+  <si>
+    <t>360.00 (180.00+180.00)</t>
+  </si>
+  <si>
+    <t>338, 517</t>
+  </si>
+  <si>
+    <t>Neubiberg Klasse 5a</t>
+  </si>
+  <si>
+    <t>530.00 (265.00+265.00)</t>
+  </si>
+  <si>
+    <t>337, 588</t>
+  </si>
+  <si>
+    <t>Anna Nikolov</t>
+  </si>
+  <si>
+    <t>Neubiberg PUG 4</t>
+  </si>
+  <si>
+    <t>Neubiberg Klasse 1a</t>
+  </si>
+  <si>
+    <t>Adri Mali</t>
+  </si>
+  <si>
+    <t>Alex Mali</t>
+  </si>
+  <si>
+    <t>Nik Vakl Mali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max  Musterman </t>
+  </si>
+  <si>
+    <t>Alb Trif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teo Musterman </t>
+  </si>
+  <si>
+    <t>Alex Nikolov</t>
+  </si>
+  <si>
+    <t>Geo Nikolov</t>
+  </si>
+  <si>
+    <t>Aleks Hadzh</t>
+  </si>
+  <si>
+    <t>Adri Hadzh</t>
+  </si>
+  <si>
+    <t>Sim Hadzh</t>
   </si>
 </sst>
 </file>
@@ -79,10 +142,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,17 +164,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
+      <left style="thin">
+        <color auto="1"/>
       </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
+      <right style="thin">
+        <color auto="1"/>
       </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
+      <top style="thin">
+        <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -123,7 +185,7 @@
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -405,15 +467,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C5"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.5703125" customWidth="1"/>
+    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="33" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -423,49 +495,204 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2">
+        <v>530</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>540</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5">
+        <v>360</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6">
+        <v>530</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7">
+        <v>530</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8">
+        <v>530</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -475,6 +702,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="69b70055-4ccd-41e5-ba44-04aa7b40ef87">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0d7d4427-3d9a-4210-88a6-80411ae356c7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100202D4B9E3A436A44B91CC234F5A1B18B" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="faa7d1780a64debc3e5433f1993c437a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="69b70055-4ccd-41e5-ba44-04aa7b40ef87" xmlns:ns3="0d7d4427-3d9a-4210-88a6-80411ae356c7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46ac9b7ec201ca2a68a6a1e758789984" ns2:_="" ns3:_="">
     <xsd:import namespace="69b70055-4ccd-41e5-ba44-04aa7b40ef87"/>
@@ -669,17 +907,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="69b70055-4ccd-41e5-ba44-04aa7b40ef87">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0d7d4427-3d9a-4210-88a6-80411ae356c7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -690,6 +917,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6E074D9-8A3F-4B12-8FF2-84C884A0412A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="69b70055-4ccd-41e5-ba44-04aa7b40ef87"/>
+    <ds:schemaRef ds:uri="0d7d4427-3d9a-4210-88a6-80411ae356c7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98CB3CB1-47E5-4ECC-B8C0-D8BE43DCE475}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -708,17 +946,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6E074D9-8A3F-4B12-8FF2-84C884A0412A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="69b70055-4ccd-41e5-ba44-04aa7b40ef87"/>
-    <ds:schemaRef ds:uri="0d7d4427-3d9a-4210-88a6-80411ae356c7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A75E2A0C-A03D-4EF1-AA2F-BC86D3F36961}">
   <ds:schemaRefs>

</xml_diff>